<commit_message>
flake8 and data dictionary update
</commit_message>
<xml_diff>
--- a/src/obds_fhir_to_opal/datadictionary_bzkf_q4_22.xlsx
+++ b/src/obds_fhir_to_opal/datadictionary_bzkf_q4_22.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\Abteilungen\ISA\DIZ\BZKF\BZKF_Abfrage1_Q4_2023\11_23-01_24\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zieglejn\git\BZKF\diz-in-a-box\src\obds_fhir_to_opal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B83371-06E5-4E85-86C7-1FC94BC15F19}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A51B54-019B-4C36-9B34-1D0047090BA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="414" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="93">
   <si>
     <t>index</t>
   </si>
@@ -300,6 +300,15 @@
   </si>
   <si>
     <t>patID</t>
+  </si>
+  <si>
+    <t>conditiondate_year</t>
+  </si>
+  <si>
+    <t>Condition Date Year</t>
+  </si>
+  <si>
+    <t>Diagnosejahr</t>
   </si>
 </sst>
 </file>
@@ -742,10 +751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,7 +1008,7 @@
         <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
@@ -1010,18 +1019,18 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="4" t="s">
-        <v>3</v>
+      <c r="H8" s="4">
+        <v>0</v>
       </c>
       <c r="I8" s="3"/>
-      <c r="J8" s="2">
+      <c r="J8" s="4">
         <v>1</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>17</v>
+        <v>91</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>18</v>
+        <v>92</v>
       </c>
       <c r="M8" s="5"/>
     </row>
@@ -1030,10 +1039,10 @@
         <v>72</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>2</v>
@@ -1041,159 +1050,164 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="4">
-        <v>0</v>
+      <c r="H9" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="2">
         <v>1</v>
       </c>
       <c r="K9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9" s="5"/>
+    </row>
+    <row r="10" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="4">
+        <v>0</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="2">
+        <v>1</v>
+      </c>
+      <c r="K10" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="L10" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="M9" s="5" t="s">
+      <c r="M10" s="5" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" t="s">
-        <v>21</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I10" t="s">
-        <v>21</v>
-      </c>
-      <c r="J10" s="4">
-        <v>1</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M10" s="7"/>
     </row>
     <row r="11" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="4">
+        <v>1</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M11" s="7"/>
+    </row>
+    <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H11" s="4">
+      <c r="C12" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="4">
         <v>0</v>
       </c>
-      <c r="J11" s="4">
-        <v>1</v>
-      </c>
-      <c r="K11" s="8" t="s">
+      <c r="J12" s="4">
+        <v>1</v>
+      </c>
+      <c r="K12" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="L11" s="9" t="s">
+      <c r="L12" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="M11" s="16"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="M12" s="16"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" t="s">
         <v>68</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="C13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
         <v>21</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F13" t="s">
         <v>21</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G13" t="s">
         <v>25</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I13" t="s">
         <v>21</v>
       </c>
-      <c r="J12" s="4">
-        <v>1</v>
-      </c>
-      <c r="K12" s="8" t="s">
+      <c r="J13" s="4">
+        <v>1</v>
+      </c>
+      <c r="K13" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="L12" s="9" t="s">
+      <c r="L13" s="9" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" t="s">
         <v>79</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H13" s="4">
-        <v>0</v>
-      </c>
-      <c r="J13" s="4">
-        <v>1</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="L13" s="9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B14" t="s">
-        <v>81</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>1</v>
@@ -1208,10 +1222,10 @@
         <v>1</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="L14" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1219,7 +1233,7 @@
         <v>72</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>1</v>
@@ -1227,26 +1241,17 @@
       <c r="D15" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E15" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" t="s">
-        <v>21</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I15" t="s">
-        <v>21</v>
+      <c r="H15" s="4">
+        <v>0</v>
       </c>
       <c r="J15" s="4">
         <v>1</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>29</v>
+        <v>82</v>
       </c>
       <c r="L15" s="9" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1254,34 +1259,42 @@
         <v>72</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" t="s">
+        <v>21</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="I16" t="s">
+        <v>21</v>
+      </c>
       <c r="J16" s="4">
         <v>1</v>
       </c>
-      <c r="K16" s="3" t="s">
-        <v>32</v>
+      <c r="K16" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="L16" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="M16" s="8"/>
+        <v>30</v>
+      </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>5</v>
@@ -1296,10 +1309,10 @@
         <v>1</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="L17" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="M17" s="8"/>
     </row>
@@ -1308,21 +1321,25 @@
         <v>72</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H18" s="4"/>
-      <c r="J18" s="4"/>
+      <c r="H18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J18" s="4">
+        <v>1</v>
+      </c>
       <c r="K18" s="3" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="L18" s="9" t="s">
-        <v>71</v>
+        <v>36</v>
       </c>
       <c r="M18" s="8"/>
     </row>
@@ -1331,25 +1348,21 @@
         <v>72</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>13</v>
+        <v>69</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>1</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H19" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J19" s="4">
-        <v>1</v>
-      </c>
+      <c r="H19" s="4"/>
+      <c r="J19" s="4"/>
       <c r="K19" s="3" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="L19" s="9" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="M19" s="8"/>
     </row>
@@ -1358,10 +1371,10 @@
         <v>72</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>1</v>
+        <v>37</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>2</v>
@@ -1373,19 +1386,19 @@
         <v>1</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="L20" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
+      </c>
+      <c r="L20" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="M20" s="8"/>
     </row>
-    <row r="21" spans="1:13" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>1</v>
@@ -1403,44 +1416,71 @@
         <v>41</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="M21" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="M21" s="8"/>
+    </row>
+    <row r="22" spans="1:13" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>13</v>
+        <v>43</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>1</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>2</v>
-      </c>
-      <c r="E22" t="s">
-        <v>21</v>
-      </c>
-      <c r="F22" t="s">
-        <v>21</v>
       </c>
       <c r="H22" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" s="4">
+        <v>1</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="M22" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" t="s">
         <v>21</v>
       </c>
-      <c r="J22" s="4">
-        <v>1</v>
-      </c>
-      <c r="K22" s="8" t="s">
+      <c r="F23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I23" t="s">
+        <v>21</v>
+      </c>
+      <c r="J23" s="4">
+        <v>1</v>
+      </c>
+      <c r="K23" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="L22" s="8" t="s">
+      <c r="L23" s="8" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: add column conditiondate year for filtering in data shield (#169)
* add column conditiondate year for safety check in data shield

* flake8 and data dictionary update
</commit_message>
<xml_diff>
--- a/src/obds_fhir_to_opal/datadictionary_bzkf_q4_22.xlsx
+++ b/src/obds_fhir_to_opal/datadictionary_bzkf_q4_22.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\Abteilungen\ISA\DIZ\BZKF\BZKF_Abfrage1_Q4_2023\11_23-01_24\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zieglejn\git\BZKF\diz-in-a-box\src\obds_fhir_to_opal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B83371-06E5-4E85-86C7-1FC94BC15F19}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A51B54-019B-4C36-9B34-1D0047090BA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="414" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="93">
   <si>
     <t>index</t>
   </si>
@@ -300,6 +300,15 @@
   </si>
   <si>
     <t>patID</t>
+  </si>
+  <si>
+    <t>conditiondate_year</t>
+  </si>
+  <si>
+    <t>Condition Date Year</t>
+  </si>
+  <si>
+    <t>Diagnosejahr</t>
   </si>
 </sst>
 </file>
@@ -742,10 +751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,7 +1008,7 @@
         <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
@@ -1010,18 +1019,18 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="4" t="s">
-        <v>3</v>
+      <c r="H8" s="4">
+        <v>0</v>
       </c>
       <c r="I8" s="3"/>
-      <c r="J8" s="2">
+      <c r="J8" s="4">
         <v>1</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>17</v>
+        <v>91</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>18</v>
+        <v>92</v>
       </c>
       <c r="M8" s="5"/>
     </row>
@@ -1030,10 +1039,10 @@
         <v>72</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>2</v>
@@ -1041,159 +1050,164 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="4">
-        <v>0</v>
+      <c r="H9" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="2">
         <v>1</v>
       </c>
       <c r="K9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9" s="5"/>
+    </row>
+    <row r="10" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="4">
+        <v>0</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="2">
+        <v>1</v>
+      </c>
+      <c r="K10" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="L10" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="M9" s="5" t="s">
+      <c r="M10" s="5" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" t="s">
-        <v>21</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I10" t="s">
-        <v>21</v>
-      </c>
-      <c r="J10" s="4">
-        <v>1</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M10" s="7"/>
     </row>
     <row r="11" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="4">
+        <v>1</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M11" s="7"/>
+    </row>
+    <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H11" s="4">
+      <c r="C12" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="4">
         <v>0</v>
       </c>
-      <c r="J11" s="4">
-        <v>1</v>
-      </c>
-      <c r="K11" s="8" t="s">
+      <c r="J12" s="4">
+        <v>1</v>
+      </c>
+      <c r="K12" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="L11" s="9" t="s">
+      <c r="L12" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="M11" s="16"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="M12" s="16"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" t="s">
         <v>68</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="C13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
         <v>21</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F13" t="s">
         <v>21</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G13" t="s">
         <v>25</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I13" t="s">
         <v>21</v>
       </c>
-      <c r="J12" s="4">
-        <v>1</v>
-      </c>
-      <c r="K12" s="8" t="s">
+      <c r="J13" s="4">
+        <v>1</v>
+      </c>
+      <c r="K13" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="L12" s="9" t="s">
+      <c r="L13" s="9" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" t="s">
         <v>79</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H13" s="4">
-        <v>0</v>
-      </c>
-      <c r="J13" s="4">
-        <v>1</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="L13" s="9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B14" t="s">
-        <v>81</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>1</v>
@@ -1208,10 +1222,10 @@
         <v>1</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="L14" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1219,7 +1233,7 @@
         <v>72</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>1</v>
@@ -1227,26 +1241,17 @@
       <c r="D15" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E15" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" t="s">
-        <v>21</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I15" t="s">
-        <v>21</v>
+      <c r="H15" s="4">
+        <v>0</v>
       </c>
       <c r="J15" s="4">
         <v>1</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>29</v>
+        <v>82</v>
       </c>
       <c r="L15" s="9" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1254,34 +1259,42 @@
         <v>72</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" t="s">
+        <v>21</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="I16" t="s">
+        <v>21</v>
+      </c>
       <c r="J16" s="4">
         <v>1</v>
       </c>
-      <c r="K16" s="3" t="s">
-        <v>32</v>
+      <c r="K16" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="L16" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="M16" s="8"/>
+        <v>30</v>
+      </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>5</v>
@@ -1296,10 +1309,10 @@
         <v>1</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="L17" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="M17" s="8"/>
     </row>
@@ -1308,21 +1321,25 @@
         <v>72</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H18" s="4"/>
-      <c r="J18" s="4"/>
+      <c r="H18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J18" s="4">
+        <v>1</v>
+      </c>
       <c r="K18" s="3" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="L18" s="9" t="s">
-        <v>71</v>
+        <v>36</v>
       </c>
       <c r="M18" s="8"/>
     </row>
@@ -1331,25 +1348,21 @@
         <v>72</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>13</v>
+        <v>69</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>1</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H19" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J19" s="4">
-        <v>1</v>
-      </c>
+      <c r="H19" s="4"/>
+      <c r="J19" s="4"/>
       <c r="K19" s="3" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="L19" s="9" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="M19" s="8"/>
     </row>
@@ -1358,10 +1371,10 @@
         <v>72</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>1</v>
+        <v>37</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>2</v>
@@ -1373,19 +1386,19 @@
         <v>1</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="L20" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
+      </c>
+      <c r="L20" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="M20" s="8"/>
     </row>
-    <row r="21" spans="1:13" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>1</v>
@@ -1403,44 +1416,71 @@
         <v>41</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="M21" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="M21" s="8"/>
+    </row>
+    <row r="22" spans="1:13" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>13</v>
+        <v>43</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>1</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>2</v>
-      </c>
-      <c r="E22" t="s">
-        <v>21</v>
-      </c>
-      <c r="F22" t="s">
-        <v>21</v>
       </c>
       <c r="H22" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" s="4">
+        <v>1</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="M22" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" t="s">
         <v>21</v>
       </c>
-      <c r="J22" s="4">
-        <v>1</v>
-      </c>
-      <c r="K22" s="8" t="s">
+      <c r="F23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I23" t="s">
+        <v>21</v>
+      </c>
+      <c r="J23" s="4">
+        <v>1</v>
+      </c>
+      <c r="K23" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="L22" s="8" t="s">
+      <c r="L23" s="8" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
corrected table name (#171)
</commit_message>
<xml_diff>
--- a/src/obds_fhir_to_opal/datadictionary_bzkf_q4_22.xlsx
+++ b/src/obds_fhir_to_opal/datadictionary_bzkf_q4_22.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zieglejn\git\BZKF\diz-in-a-box\src\obds_fhir_to_opal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\Abteilungen\ISA\DIZ\BZKF\BZKF_Abfrage1_Q4_2023\11_23-01_24\DQA-Datenvergleich\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A51B54-019B-4C36-9B34-1D0047090BA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F048FBB4-B109-415D-BB74-F5C3B085552D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="414" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="91">
   <si>
     <t>index</t>
   </si>
@@ -285,12 +285,6 @@
   </si>
   <si>
     <t>Altergruppierung klein 0-14, 15-19, 20-24, 25-29, 30-34, 35-39, 40-44, 45-49, 50-54, 55-59...80-84, 85+</t>
-  </si>
-  <si>
-    <t>bzkf_q4_23</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
   <si>
     <t>Patient FHIR Resource Identifier</t>
@@ -753,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,19 +864,19 @@
         <v>1</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M3" s="5"/>
     </row>
     <row r="4" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
@@ -894,17 +888,17 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="4" t="s">
-        <v>86</v>
+        <v>3</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="2">
         <v>1</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="M4" s="5"/>
     </row>
@@ -1008,7 +1002,7 @@
         <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
@@ -1027,10 +1021,10 @@
         <v>1</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="M8" s="5"/>
     </row>

</xml_diff>